<commit_message>
Now it is possible to add multiplefiles using single dialog call. Removed skipping first row in xlsx (when there is a title)
</commit_message>
<xml_diff>
--- a/src/main/python/science/samples/1_6.xlsx
+++ b/src/main/python/science/samples/1_6.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1EDA82C-5166-D74A-B3EC-5AD60CD82553}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -192,7 +193,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -503,16 +504,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -526,7 +527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -540,7 +541,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -554,7 +555,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -568,7 +569,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -582,7 +583,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -596,7 +597,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -610,7 +611,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -624,7 +625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -638,7 +639,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -652,7 +653,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -666,7 +667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -680,7 +681,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -694,7 +695,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -708,7 +709,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -722,7 +723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -736,7 +737,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -750,7 +751,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -764,7 +765,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -778,7 +779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -792,7 +793,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -806,7 +807,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -820,7 +821,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -834,7 +835,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -848,7 +849,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -862,7 +863,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -876,7 +877,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -890,7 +891,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -904,7 +905,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -918,7 +919,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -932,7 +933,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -946,7 +947,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -960,7 +961,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -974,7 +975,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -988,7 +989,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -1002,7 +1003,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>24</v>
       </c>
@@ -1016,7 +1017,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>25</v>
       </c>
@@ -1030,7 +1031,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>26</v>
       </c>
@@ -1044,7 +1045,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -1058,7 +1059,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>13</v>
       </c>
@@ -1072,7 +1073,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>27</v>
       </c>
@@ -1086,7 +1087,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>28</v>
       </c>
@@ -1100,7 +1101,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -1114,7 +1115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -1128,7 +1129,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -1142,7 +1143,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -1156,7 +1157,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>2</v>
       </c>
@@ -1170,7 +1171,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>3</v>
       </c>
@@ -1184,7 +1185,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>11</v>
       </c>
@@ -1198,7 +1199,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>29</v>
       </c>
@@ -1212,7 +1213,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>29</v>
       </c>
@@ -1226,7 +1227,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>30</v>
       </c>
@@ -1240,7 +1241,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -1254,7 +1255,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>22</v>
       </c>
@@ -1268,7 +1269,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -1282,7 +1283,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -1296,7 +1297,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>31</v>
       </c>
@@ -1310,7 +1311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>32</v>
       </c>
@@ -1324,7 +1325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>13</v>
       </c>
@@ -1338,7 +1339,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>6</v>
       </c>

</xml_diff>